<commit_message>
nomenclatura y  archivo del Modulo s_portal-interno v2
nomenclatura y  archivo del Modulo s_portal-interno v2
</commit_message>
<xml_diff>
--- a/00-Documentacion/nomenclatura.xlsx
+++ b/00-Documentacion/nomenclatura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_hub_LogisLJC\migracion\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31954445-7DC7-4F8F-AFD5-8BD94F11B5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05836FBC-0B47-41A4-AC2C-852E1C5D2CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{595E4830-43DA-4794-BED7-741D567A698A}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="16305" windowHeight="9975" xr2:uid="{595E4830-43DA-4794-BED7-741D567A698A}"/>
   </bookViews>
   <sheets>
     <sheet name="generico" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>T</t>
   </si>
@@ -75,9 +75,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>ic</t>
-  </si>
-  <si>
     <t>usua</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Store</t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sistema </t>
   </si>
   <si>
@@ -142,6 +136,15 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Funcion</t>
+  </si>
+  <si>
+    <t>Fn</t>
+  </si>
+  <si>
+    <t>Sp</t>
   </si>
 </sst>
 </file>
@@ -243,13 +246,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,12 +264,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FABF14-C099-4BEC-AF29-2D66042615C1}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,40 +606,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -662,32 +666,30 @@
         <v>3</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="M2" s="4" t="s">
-        <v>19</v>
+      <c r="M2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
@@ -698,36 +700,34 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>CONCATENATE(B3,C3,D3,E3,F3,G3,H3,I3)</f>
-        <v>Tx_ic_C_usua</v>
-      </c>
-      <c r="M3" s="5"/>
+        <v>Tx__C_usua</v>
+      </c>
+      <c r="M3" s="7"/>
       <c r="N3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
         <v>2</v>
@@ -738,86 +738,120 @@
       </c>
       <c r="J4" s="2" t="str">
         <f>CONCATENATE(B4,C4,D4,E4,F4,G4,H4,I4)</f>
-        <v>SPx_icCUsuario</v>
-      </c>
-      <c r="M4" s="6"/>
+        <v>Spx_CUsuario</v>
+      </c>
+      <c r="M4" s="8"/>
       <c r="N4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="9" t="s">
-        <v>31</v>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="J5" s="2" t="str">
         <f>CONCATENATE(B5,C5,D5,E5,F5,G5,H5,I5)</f>
-        <v>exNom. de la variable</v>
+        <v>Fnx_CUsuario</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>20</v>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6)</f>
+        <v>exNom. de la variable</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="2" t="str">
-        <f t="shared" ref="J6:J7" si="0">CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6)</f>
-        <v>sxNom. de la variable</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="11"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="9" t="s">
-        <v>31</v>
+      <c r="I7" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="J7" s="2" t="str">
+        <f t="shared" ref="J7:J8" si="0">CONCATENATE(B7,C7,D7,E7,F7,G7,H7,I7)</f>
+        <v>sxNom. de la variable</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>vNom. de la variable</v>
       </c>
@@ -825,7 +859,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="M2:M4"/>
-    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>